<commit_message>
SupervisorLogin test, Create Interaction
</commit_message>
<xml_diff>
--- a/resources/excels/CG.xlsx
+++ b/resources/excels/CG.xlsx
@@ -528,12 +528,6 @@
     <t>SIM Bar Unbar</t>
   </si>
   <si>
-    <t>SIM Lost</t>
-  </si>
-  <si>
-    <t>SIM Broken</t>
-  </si>
-  <si>
     <t>Queue Name</t>
   </si>
   <si>
@@ -1151,6 +1145,12 @@
   <si>
     <t>Post balance
 (CFA)</t>
+  </si>
+  <si>
+    <t>Customer Request</t>
+  </si>
+  <si>
+    <t>Customer wants to use Pay as you go</t>
   </si>
 </sst>
 </file>
@@ -1444,7 +1444,7 @@
         <xdr:cNvPr id="3" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{954E16FB-6A94-A343-90CA-E894AD77BEF0}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{954E16FB-6A94-A343-90CA-E894AD77BEF0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1487,7 +1487,7 @@
         <xdr:cNvPr id="4" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{954E16FB-6A94-A343-90CA-E894AD77BEF0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{954E16FB-6A94-A343-90CA-E894AD77BEF0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1530,7 +1530,7 @@
         <xdr:cNvPr id="5" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{954E16FB-6A94-A343-90CA-E894AD77BEF0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{954E16FB-6A94-A343-90CA-E894AD77BEF0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1573,7 +1573,7 @@
         <xdr:cNvPr id="6" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{954E16FB-6A94-A343-90CA-E894AD77BEF0}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{954E16FB-6A94-A343-90CA-E894AD77BEF0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1616,7 +1616,7 @@
         <xdr:cNvPr id="7" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{954E16FB-6A94-A343-90CA-E894AD77BEF0}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{954E16FB-6A94-A343-90CA-E894AD77BEF0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1971,10 +1971,10 @@
         <v>14</v>
       </c>
       <c r="P1" s="11" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="Q1" s="11" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -1982,7 +1982,7 @@
         <v>2390932</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>109</v>
@@ -2001,13 +2001,13 @@
       <c r="M2" s="11"/>
       <c r="N2" s="11"/>
       <c r="O2" s="11" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="P2" s="11" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="Q2" s="11" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -2015,7 +2015,7 @@
         <v>2394650</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>110</v>
@@ -2035,7 +2035,7 @@
       <c r="N3" s="11"/>
       <c r="O3" s="11"/>
       <c r="P3" s="11" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="Q3" s="11"/>
     </row>
@@ -2044,7 +2044,7 @@
         <v>2388008</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>111</v>
@@ -2064,7 +2064,7 @@
       <c r="N4" s="11"/>
       <c r="O4" s="11"/>
       <c r="P4" s="11" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="Q4" s="11"/>
     </row>
@@ -2073,7 +2073,7 @@
         <v>2390932</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>112</v>
@@ -2093,7 +2093,7 @@
       <c r="N5" s="11"/>
       <c r="O5" s="11"/>
       <c r="P5" s="11" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="Q5" s="11"/>
     </row>
@@ -2356,13 +2356,13 @@
     </row>
     <row r="2" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
+        <v>314</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>315</v>
+      </c>
+      <c r="C2" s="28" t="s">
         <v>316</v>
-      </c>
-      <c r="B2" s="28" t="s">
-        <v>317</v>
-      </c>
-      <c r="C2" s="28" t="s">
-        <v>318</v>
       </c>
       <c r="D2" s="28" t="s">
         <v>149</v>
@@ -2380,7 +2380,7 @@
         <v>148</v>
       </c>
       <c r="I2" s="28" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -2397,7 +2397,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2435,13 +2435,13 @@
         <v>159</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="J1" s="26" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -2449,10 +2449,10 @@
         <v>160</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>161</v>
+        <v>366</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>162</v>
+        <v>367</v>
       </c>
       <c r="J2" s="25" t="b">
         <v>1</v>
@@ -2460,7 +2460,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B3"/>
       <c r="C3"/>
@@ -2469,10 +2469,10 @@
       <c r="F3"/>
       <c r="G3"/>
       <c r="H3" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="I3" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="J3" s="25" t="b">
         <v>0</v>
@@ -2480,7 +2480,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B4" s="25"/>
       <c r="C4" s="25"/>
@@ -2496,7 +2496,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B5" s="25"/>
       <c r="C5" s="25"/>
@@ -2512,7 +2512,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B6" s="25"/>
       <c r="C6" s="25"/>
@@ -2528,7 +2528,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B7" s="25"/>
       <c r="C7" s="25"/>
@@ -2544,7 +2544,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B8" s="25"/>
       <c r="C8" s="25"/>
@@ -2560,7 +2560,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B9" s="25"/>
       <c r="C9" s="25"/>
@@ -2576,7 +2576,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B10" s="25"/>
       <c r="C10" s="25"/>
@@ -2592,7 +2592,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B11" s="25"/>
       <c r="C11" s="25"/>
@@ -2608,7 +2608,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="25" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B12" s="25"/>
       <c r="C12" s="25"/>
@@ -2624,7 +2624,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B13" s="25"/>
       <c r="C13" s="25"/>
@@ -2663,42 +2663,42 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="C1" s="18" t="s">
         <v>163</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="D1" s="18" t="s">
         <v>164</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="E1" s="18" t="s">
         <v>165</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="F1" s="18" t="s">
         <v>166</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="G1" s="18" t="s">
         <v>167</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="H1" s="18" t="s">
         <v>168</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="I1" s="18" t="s">
         <v>169</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="J1" s="18" t="s">
         <v>170</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="K1" s="18" t="s">
         <v>171</v>
-      </c>
-      <c r="J1" s="18" t="s">
-        <v>172</v>
-      </c>
-      <c r="K1" s="18" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B2" s="18" t="s">
         <v>57</v>
@@ -2719,7 +2719,7 @@
     </row>
     <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B3" s="18" t="s">
         <v>57</v>
@@ -2824,7 +2824,7 @@
     </row>
     <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>57</v>
@@ -2845,7 +2845,7 @@
     </row>
     <row r="9" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>57</v>
@@ -2866,7 +2866,7 @@
     </row>
     <row r="10" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="27" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B10" s="18" t="s">
         <v>57</v>
@@ -2914,12 +2914,12 @@
         <v>134</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>70</v>
@@ -2933,7 +2933,7 @@
         <v>70</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C3" s="15" t="b">
         <v>1</v>
@@ -2963,161 +2963,161 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
+        <v>251</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>253</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>254</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="C2" s="15" t="s">
         <v>256</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>257</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
+        <v>257</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>258</v>
+      </c>
+      <c r="C3" s="15" t="s">
         <v>259</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>260</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="C4" s="15" t="s">
         <v>262</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>263</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
+        <v>263</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>264</v>
+      </c>
+      <c r="C5" s="15" t="s">
         <v>265</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>266</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C6" s="24"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
+        <v>268</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>269</v>
+      </c>
+      <c r="C7" s="15" t="s">
         <v>270</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>271</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
+        <v>271</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>272</v>
+      </c>
+      <c r="C8" s="15" t="s">
         <v>273</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>274</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
+        <v>274</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>275</v>
+      </c>
+      <c r="C9" s="15" t="s">
         <v>276</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>277</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
+        <v>277</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>278</v>
+      </c>
+      <c r="C10" s="15" t="s">
         <v>279</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>280</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
+        <v>280</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>281</v>
+      </c>
+      <c r="C11" s="15" t="s">
         <v>282</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>283</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
+        <v>283</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="C12" s="15" t="s">
         <v>285</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>286</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C13" s="24"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C14" s="24"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
+        <v>290</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>291</v>
+      </c>
+      <c r="C15" s="15" t="s">
         <v>292</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>293</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>294</v>
       </c>
     </row>
   </sheetData>
@@ -3231,16 +3231,16 @@
         <v>24</v>
       </c>
       <c r="J1" s="21" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="K1" s="21" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="L1" s="11" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="M1" s="11" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -3248,7 +3248,7 @@
         <v>68</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>78</v>
@@ -3287,7 +3287,7 @@
         <v>85</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
@@ -3302,7 +3302,7 @@
         <v>86</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>84</v>
@@ -3311,7 +3311,7 @@
         <v>87</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>81</v>
@@ -3350,7 +3350,7 @@
         <v>93</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="J5" s="11"/>
       <c r="K5" s="11"/>
@@ -3463,22 +3463,22 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
+        <v>181</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>361</v>
+      </c>
+      <c r="D10" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="E10" s="11" t="s">
         <v>184</v>
       </c>
-      <c r="C10" s="11" t="s">
-        <v>363</v>
-      </c>
-      <c r="D10" s="11" t="s">
+      <c r="F10" s="11" t="s">
         <v>185</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>187</v>
       </c>
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
@@ -3490,22 +3490,22 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="C11" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="D11" s="11" t="s">
         <v>189</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="E11" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="F11" s="11" t="s">
         <v>191</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>193</v>
       </c>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
@@ -3517,28 +3517,28 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="C12" s="11" t="s">
         <v>194</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="D12" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="E12" s="11" t="s">
         <v>196</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="F12" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="G12" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="F12" s="11" t="s">
+      <c r="H12" s="11" t="s">
         <v>199</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>200</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>201</v>
       </c>
       <c r="I12" s="11"/>
       <c r="J12" s="11"/>
@@ -3548,19 +3548,19 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>77</v>
       </c>
       <c r="C13" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="E13" s="11" t="s">
         <v>203</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>204</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>205</v>
       </c>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
@@ -3573,10 +3573,10 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>84</v>
@@ -3585,22 +3585,22 @@
         <v>87</v>
       </c>
       <c r="E14" s="22" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F14" s="21" t="s">
         <v>81</v>
       </c>
       <c r="G14" s="21" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H14" s="21" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="I14" s="21" t="s">
         <v>106</v>
       </c>
       <c r="J14" s="21" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="K14" s="21" t="s">
         <v>93</v>
@@ -3610,7 +3610,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>26</v>
@@ -3622,13 +3622,13 @@
         <v>85</v>
       </c>
       <c r="E15" s="21" t="s">
+        <v>210</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="G15" s="11" t="s">
         <v>212</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>213</v>
-      </c>
-      <c r="G15" s="11" t="s">
-        <v>214</v>
       </c>
       <c r="H15" s="11" t="s">
         <v>87</v>
@@ -3641,16 +3641,16 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
+        <v>213</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="C16" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="D16" s="11" t="s">
         <v>216</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>217</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>218</v>
       </c>
       <c r="E16" s="11" t="s">
         <v>153</v>
@@ -3666,19 +3666,19 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
+        <v>219</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>220</v>
+      </c>
+      <c r="C17" s="21" t="s">
         <v>221</v>
       </c>
-      <c r="B17" s="21" t="s">
+      <c r="D17" s="21" t="s">
         <v>222</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="E17" s="21" t="s">
         <v>223</v>
-      </c>
-      <c r="D17" s="21" t="s">
-        <v>224</v>
-      </c>
-      <c r="E17" s="21" t="s">
-        <v>225</v>
       </c>
       <c r="F17" s="11"/>
       <c r="G17" s="11"/>
@@ -3691,19 +3691,19 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>231</v>
+      </c>
+      <c r="C18" s="21" t="s">
         <v>232</v>
       </c>
-      <c r="B18" s="21" t="s">
+      <c r="D18" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="C18" s="21" t="s">
+      <c r="E18" s="21" t="s">
         <v>234</v>
-      </c>
-      <c r="D18" s="21" t="s">
-        <v>235</v>
-      </c>
-      <c r="E18" s="21" t="s">
-        <v>236</v>
       </c>
       <c r="F18" s="11" t="s">
         <v>153</v>
@@ -3718,66 +3718,66 @@
     </row>
     <row r="19" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="21" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C19" s="21" t="s">
         <v>79</v>
       </c>
       <c r="D19" s="21" t="s">
+        <v>236</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>237</v>
+      </c>
+      <c r="F19" s="21" t="s">
         <v>238</v>
       </c>
-      <c r="E19" s="21" t="s">
+      <c r="G19" s="21" t="s">
         <v>239</v>
-      </c>
-      <c r="F19" s="21" t="s">
-        <v>240</v>
-      </c>
-      <c r="G19" s="21" t="s">
-        <v>241</v>
       </c>
       <c r="H19" s="21" t="s">
         <v>80</v>
       </c>
       <c r="I19" s="23" t="s">
+        <v>363</v>
+      </c>
+      <c r="J19" s="23" t="s">
+        <v>364</v>
+      </c>
+      <c r="K19" s="23" t="s">
         <v>365</v>
-      </c>
-      <c r="J19" s="23" t="s">
-        <v>366</v>
-      </c>
-      <c r="K19" s="23" t="s">
-        <v>367</v>
       </c>
       <c r="L19" s="21" t="s">
         <v>81</v>
       </c>
       <c r="M19" s="21" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C20" s="11" t="s">
         <v>84</v>
       </c>
       <c r="D20" s="21" t="s">
+        <v>243</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>244</v>
+      </c>
+      <c r="F20" s="21" t="s">
         <v>245</v>
       </c>
-      <c r="E20" s="21" t="s">
+      <c r="G20" s="21" t="s">
         <v>246</v>
-      </c>
-      <c r="F20" s="21" t="s">
-        <v>247</v>
-      </c>
-      <c r="G20" s="21" t="s">
-        <v>248</v>
       </c>
       <c r="H20" s="11"/>
       <c r="I20" s="11"/>
@@ -3788,34 +3788,34 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
+        <v>347</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>348</v>
+      </c>
+      <c r="C21" s="11" t="s">
         <v>349</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="D21" s="11" t="s">
         <v>350</v>
       </c>
-      <c r="C21" s="11" t="s">
-        <v>351</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>352</v>
-      </c>
       <c r="E21" s="11" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F21" s="11" t="s">
         <v>106</v>
       </c>
       <c r="G21" s="11" t="s">
+        <v>351</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>352</v>
+      </c>
+      <c r="I21" s="11" t="s">
         <v>353</v>
       </c>
-      <c r="H21" s="11" t="s">
+      <c r="J21" s="11" t="s">
         <v>354</v>
-      </c>
-      <c r="I21" s="11" t="s">
-        <v>355</v>
-      </c>
-      <c r="J21" s="11" t="s">
-        <v>356</v>
       </c>
       <c r="K21" s="11"/>
       <c r="L21" s="11"/>
@@ -3823,22 +3823,22 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
+        <v>355</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>356</v>
+      </c>
+      <c r="C22" s="11" t="s">
         <v>357</v>
       </c>
-      <c r="B22" s="11" t="s">
-        <v>358</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>359</v>
-      </c>
       <c r="D22" s="11" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E22" s="11" t="s">
         <v>106</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="G22" s="11" t="s">
         <v>153</v>
@@ -3937,25 +3937,25 @@
         <v>32</v>
       </c>
       <c r="X1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="Y1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="Z1" t="s">
         <v>32</v>
       </c>
       <c r="AA1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="AB1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="AC1" t="s">
         <v>32</v>
       </c>
       <c r="AD1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="AE1" t="s">
         <v>34</v>
@@ -3964,7 +3964,7 @@
         <v>32</v>
       </c>
       <c r="AG1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="AH1" t="s">
         <v>36</v>
@@ -3973,7 +3973,7 @@
         <v>32</v>
       </c>
       <c r="AJ1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="AK1" t="s">
         <v>38</v>
@@ -3982,7 +3982,7 @@
         <v>32</v>
       </c>
       <c r="AM1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="AN1" t="s">
         <v>40</v>
@@ -3991,7 +3991,7 @@
         <v>32</v>
       </c>
       <c r="AP1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="AQ1" t="s">
         <v>108</v>
@@ -4000,10 +4000,10 @@
         <v>32</v>
       </c>
       <c r="AS1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="AT1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="AU1" t="s">
         <v>32</v>
@@ -4015,25 +4015,25 @@
         <v>42</v>
       </c>
       <c r="AX1" t="s">
+        <v>174</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>175</v>
+      </c>
+      <c r="AZ1" t="s">
         <v>176</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="BA1" t="s">
         <v>177</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BB1" t="s">
         <v>178</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BC1" t="s">
         <v>179</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BD1" t="s">
         <v>180</v>
-      </c>
-      <c r="BC1" t="s">
-        <v>181</v>
-      </c>
-      <c r="BD1" t="s">
-        <v>182</v>
       </c>
       <c r="BE1" t="s">
         <v>43</v>
@@ -4050,46 +4050,46 @@
         <v>129</v>
       </c>
       <c r="B2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C2" t="s">
+        <v>321</v>
+      </c>
+      <c r="D2" t="s">
+        <v>328</v>
+      </c>
+      <c r="E2" t="s">
         <v>329</v>
       </c>
-      <c r="C2" t="s">
-        <v>323</v>
-      </c>
-      <c r="D2" t="s">
-        <v>330</v>
-      </c>
-      <c r="E2" t="s">
-        <v>331</v>
-      </c>
       <c r="F2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="G2" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="H2" t="s">
         <v>67</v>
       </c>
       <c r="I2" s="30" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="J2" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="K2" t="s">
         <v>67</v>
       </c>
       <c r="L2" s="30" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="M2" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="N2" t="s">
         <v>67</v>
       </c>
       <c r="AV2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="AW2">
         <v>0.5</v>
@@ -4098,10 +4098,10 @@
         <v>0.5</v>
       </c>
       <c r="BE2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="BF2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
   </sheetData>
@@ -4201,25 +4201,25 @@
         <v>32</v>
       </c>
       <c r="X1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="Y1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="Z1" t="s">
         <v>32</v>
       </c>
       <c r="AA1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="AB1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="AC1" t="s">
         <v>32</v>
       </c>
       <c r="AD1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="AE1" t="s">
         <v>34</v>
@@ -4228,7 +4228,7 @@
         <v>32</v>
       </c>
       <c r="AG1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="AH1" t="s">
         <v>36</v>
@@ -4237,7 +4237,7 @@
         <v>32</v>
       </c>
       <c r="AJ1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="AK1" t="s">
         <v>38</v>
@@ -4246,7 +4246,7 @@
         <v>32</v>
       </c>
       <c r="AM1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="AN1" t="s">
         <v>40</v>
@@ -4255,7 +4255,7 @@
         <v>32</v>
       </c>
       <c r="AP1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="AQ1" t="s">
         <v>108</v>
@@ -4264,10 +4264,10 @@
         <v>32</v>
       </c>
       <c r="AS1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="AT1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="AU1" t="s">
         <v>32</v>
@@ -4279,25 +4279,25 @@
         <v>42</v>
       </c>
       <c r="AX1" t="s">
+        <v>174</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>175</v>
+      </c>
+      <c r="AZ1" t="s">
         <v>176</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="BA1" t="s">
         <v>177</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BB1" t="s">
         <v>178</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BC1" t="s">
         <v>179</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BD1" t="s">
         <v>180</v>
-      </c>
-      <c r="BC1" t="s">
-        <v>181</v>
-      </c>
-      <c r="BD1" t="s">
-        <v>182</v>
       </c>
       <c r="BE1" t="s">
         <v>43</v>
@@ -4314,46 +4314,46 @@
         <v>129</v>
       </c>
       <c r="B2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C2" t="s">
+        <v>321</v>
+      </c>
+      <c r="D2" t="s">
+        <v>328</v>
+      </c>
+      <c r="E2" t="s">
         <v>329</v>
       </c>
-      <c r="C2" t="s">
-        <v>323</v>
-      </c>
-      <c r="D2" t="s">
-        <v>330</v>
-      </c>
-      <c r="E2" t="s">
-        <v>331</v>
-      </c>
       <c r="F2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="G2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="H2" t="s">
         <v>67</v>
       </c>
       <c r="I2" s="30" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="J2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="K2" t="s">
         <v>67</v>
       </c>
       <c r="L2" s="30" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="M2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="N2" t="s">
         <v>67</v>
       </c>
       <c r="AV2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="AW2">
         <v>0.5</v>
@@ -4362,10 +4362,10 @@
         <v>0.5</v>
       </c>
       <c r="BE2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="BF2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
   </sheetData>
@@ -4418,36 +4418,36 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
+        <v>320</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>321</v>
+      </c>
+      <c r="C2" s="30" t="s">
         <v>322</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="D2" s="30" t="s">
+        <v>322</v>
+      </c>
+      <c r="E2" s="30" t="s">
         <v>323</v>
-      </c>
-      <c r="C2" s="30" t="s">
-        <v>324</v>
-      </c>
-      <c r="D2" s="30" t="s">
-        <v>324</v>
-      </c>
-      <c r="E2" s="30" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="30" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B3" s="30" t="s">
         <v>69</v>
       </c>
       <c r="C3" s="30" t="s">
+        <v>324</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>325</v>
+      </c>
+      <c r="E3" s="30" t="s">
         <v>326</v>
-      </c>
-      <c r="D3" s="30" t="s">
-        <v>327</v>
-      </c>
-      <c r="E3" s="30" t="s">
-        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -4489,36 +4489,36 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
+        <v>320</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>321</v>
+      </c>
+      <c r="C2" s="29" t="s">
         <v>322</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="D2" s="29" t="s">
+        <v>322</v>
+      </c>
+      <c r="E2" s="29" t="s">
         <v>323</v>
-      </c>
-      <c r="C2" s="29" t="s">
-        <v>324</v>
-      </c>
-      <c r="D2" s="29" t="s">
-        <v>324</v>
-      </c>
-      <c r="E2" s="29" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B3" s="29" t="s">
         <v>69</v>
       </c>
       <c r="C3" s="29" t="s">
+        <v>324</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>325</v>
+      </c>
+      <c r="E3" s="29" t="s">
         <v>326</v>
-      </c>
-      <c r="D3" s="29" t="s">
-        <v>327</v>
-      </c>
-      <c r="E3" s="29" t="s">
-        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -4559,7 +4559,7 @@
         <v>126</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -4567,10 +4567,10 @@
         <v>64</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -4578,7 +4578,7 @@
         <v>65</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C4" s="27" t="s">
         <v>70</v>
@@ -4616,28 +4616,28 @@
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
       <c r="B8" s="27" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
       <c r="B9" s="27" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
       <c r="B10" s="27" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
   </sheetData>
@@ -4675,7 +4675,7 @@
         <v>52</v>
       </c>
       <c r="E1" s="31" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -4686,13 +4686,13 @@
         <v>67</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -4703,13 +4703,13 @@
         <v>67</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
   </sheetData>

</xml_diff>